<commit_message>
added a new column for the gantt chart
</commit_message>
<xml_diff>
--- a/data/tulospalvelu_gantt.xlsx
+++ b/data/tulospalvelu_gantt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeetRaju\Desktop\GitHub\Dash\SPL-dash-demo-v1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeetRaju\Desktop\GitHub\Dash\SPLDash_v1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A84E30-5750-482A-BEF8-C6AF9EAADE2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF12A79D-A39D-443F-A5AA-082D5F659E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="34">
   <si>
     <t>Tulospalvelun määrittely</t>
   </si>
@@ -92,6 +92,36 @@
   </si>
   <si>
     <t>Tasapeli</t>
+  </si>
+  <si>
+    <t>Toivoteet</t>
+  </si>
+  <si>
+    <t>Tulospalvelu</t>
+  </si>
+  <si>
+    <t>Pelipaikka</t>
+  </si>
+  <si>
+    <t>Nettisivut</t>
+  </si>
+  <si>
+    <t>Kommentti</t>
+  </si>
+  <si>
+    <t>Ei kommenttia</t>
+  </si>
+  <si>
+    <t>Tämä tehtävä epäonnistui</t>
+  </si>
+  <si>
+    <t>Tämä tehtävä ei ole vielä alkanut.</t>
+  </si>
+  <si>
+    <t>Tämä tehtävä ei edennyt suunnitellusti, koska …</t>
+  </si>
+  <si>
+    <t>Aktiivinen kehitysvaihe II</t>
   </si>
 </sst>
 </file>
@@ -933,355 +963,460 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>44075</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
+        <v>44197</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>44105</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="1">
+        <v>44228</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44105</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44228</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>44197</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44317</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>44317</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>44409</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <v>44317</v>
-      </c>
       <c r="C6" s="1">
+        <v>44378</v>
+      </c>
+      <c r="D6" s="1">
         <v>44470</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>44075</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>44166</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C8" s="1">
         <v>44228</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>44317</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>44317</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>44378</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>44256</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>44317</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>44256</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>44470</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>44256</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>44317</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>44317</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>44409</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>44105</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>44197</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>44075</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>44228</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>44228</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>44317</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>18</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>44317</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>44348</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>18</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>44348</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>44531</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>44348</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>44470</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1">
         <v>44256</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>44317</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>